<commit_message>
USD 6M YC - fix triggers
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YC6MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="24540" windowHeight="7620"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="24540" windowHeight="7620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="190">
   <si>
     <t>60Y</t>
   </si>
@@ -785,6 +785,9 @@
   </si>
   <si>
     <t>USD_YCRH_SwapsFromBasis</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1421,7 +1424,7 @@
     <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="203">
+  <cellXfs count="204">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -1848,6 +1851,7 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="10" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="28" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2187,7 +2191,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2211,19 +2215,19 @@
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="194" t="s">
+      <c r="B2" s="195" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="195"/>
-      <c r="D2" s="195"/>
-      <c r="E2" s="195"/>
-      <c r="F2" s="196"/>
-      <c r="K2" s="194" t="s">
+      <c r="C2" s="196"/>
+      <c r="D2" s="196"/>
+      <c r="E2" s="196"/>
+      <c r="F2" s="197"/>
+      <c r="K2" s="195" t="s">
         <v>167</v>
       </c>
-      <c r="L2" s="195"/>
-      <c r="M2" s="195"/>
-      <c r="N2" s="197"/>
+      <c r="L2" s="196"/>
+      <c r="M2" s="196"/>
+      <c r="N2" s="198"/>
     </row>
     <row r="3" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="59"/>
@@ -2364,12 +2368,12 @@
       </c>
       <c r="E9" s="56"/>
       <c r="F9" s="55"/>
-      <c r="K9" s="194" t="s">
+      <c r="K9" s="195" t="s">
         <v>163</v>
       </c>
-      <c r="L9" s="195"/>
-      <c r="M9" s="195"/>
-      <c r="N9" s="197"/>
+      <c r="L9" s="196"/>
+      <c r="M9" s="196"/>
+      <c r="N9" s="198"/>
     </row>
     <row r="10" spans="2:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="59"/>
@@ -2392,7 +2396,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="84">
-        <v>41655.687175925923</v>
+        <v>41655.710428240738</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="55"/>
@@ -2446,7 +2450,7 @@
       </c>
       <c r="D14" s="81" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYC6M#0003</v>
+        <v>_USDYC6M#0002</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="55"/>
@@ -2468,7 +2472,9 @@
         <f>_xll.ohRangeRetrieveError(YieldCurve)</f>
         <v/>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="194" t="s">
+        <v>189</v>
+      </c>
       <c r="F15" s="55"/>
       <c r="K15" s="118"/>
       <c r="L15" s="117" t="s">
@@ -2652,7 +2658,7 @@
       </c>
       <c r="D29" s="57" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 11th instrument (maturity: August 20th, 2014) has an invalid quote</v>
+        <v>qlPiecewiseYieldCurveData - 14th instrument (maturity: January 20th, 2016) has an invalid quote</v>
       </c>
       <c r="E29" s="56"/>
       <c r="F29" s="55"/>
@@ -2732,11 +2738,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="B1" s="198" t="s">
+      <c r="B1" s="199" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="199"/>
-      <c r="D1" s="200"/>
+      <c r="C1" s="200"/>
+      <c r="D1" s="201"/>
       <c r="E1" s="31" t="s">
         <v>74</v>
       </c>
@@ -3295,13 +3301,13 @@
       <c r="J16" s="20">
         <v>1</v>
       </c>
-      <c r="K16" s="19">
+      <c r="K16" s="19" t="e">
         <f>_xll.qlRateHelperEarliestDate($E16,Trigger)</f>
-        <v>41659</v>
-      </c>
-      <c r="L16" s="18">
+        <v>#NUM!</v>
+      </c>
+      <c r="L16" s="18" t="e">
         <f>_xll.qlRateHelperLatestDate($E16,Trigger)</f>
-        <v>41841</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
@@ -3333,13 +3339,13 @@
       <c r="J17" s="5">
         <v>1</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="4" t="e">
         <f>_xll.qlRateHelperEarliestDate($E17,Trigger)</f>
-        <v>41660</v>
-      </c>
-      <c r="L17" s="3">
+        <v>#NUM!</v>
+      </c>
+      <c r="L17" s="3" t="e">
         <f>_xll.qlRateHelperLatestDate($E17,Trigger)</f>
-        <v>41841</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
@@ -3357,9 +3363,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_1x7F</v>
       </c>
-      <c r="F18" s="13" t="e">
+      <c r="F18" s="13">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="12" t="b">
@@ -3395,9 +3401,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_2x8F</v>
       </c>
-      <c r="F19" s="13" t="e">
+      <c r="F19" s="13">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.7599999999999999E-3</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="12" t="b">
@@ -3433,9 +3439,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_3x9F</v>
       </c>
-      <c r="F20" s="13" t="e">
+      <c r="F20" s="13">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>#NUM!</v>
+        <v>3.9000000000000003E-3</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="12" t="b">
@@ -3471,9 +3477,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_4x10F</v>
       </c>
-      <c r="F21" s="13" t="e">
+      <c r="F21" s="13">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.0400000000000002E-3</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12" t="b">
@@ -3509,9 +3515,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_5x11F</v>
       </c>
-      <c r="F22" s="13" t="e">
+      <c r="F22" s="13">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.2000000000000006E-3</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="12" t="b">
@@ -3547,9 +3553,9 @@
         <f t="shared" si="0"/>
         <v>USD_YC6MRH_6x12F</v>
       </c>
-      <c r="F23" s="13" t="e">
+      <c r="F23" s="13">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>#NUM!</v>
+        <v>4.3800000000000002E-3</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="12" t="b">
@@ -3599,13 +3605,13 @@
       <c r="J24" s="12">
         <v>1</v>
       </c>
-      <c r="K24" s="11">
+      <c r="K24" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E24,Trigger)</f>
-        <v>41871</v>
-      </c>
-      <c r="L24" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L24" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E24,Trigger)</f>
-        <v>42055</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.2">
@@ -3637,13 +3643,13 @@
       <c r="J25" s="12">
         <v>1</v>
       </c>
-      <c r="K25" s="11">
+      <c r="K25" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E25,Trigger)</f>
-        <v>41904</v>
-      </c>
-      <c r="L25" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L25" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E25,Trigger)</f>
-        <v>42086</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.2">
@@ -3675,13 +3681,13 @@
       <c r="J26" s="12">
         <v>1</v>
       </c>
-      <c r="K26" s="11">
+      <c r="K26" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E26,Trigger)</f>
-        <v>41932</v>
-      </c>
-      <c r="L26" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L26" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E26,Trigger)</f>
-        <v>42114</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.2">
@@ -3713,13 +3719,13 @@
       <c r="J27" s="12">
         <v>1</v>
       </c>
-      <c r="K27" s="11">
+      <c r="K27" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E27,Trigger)</f>
-        <v>41963</v>
-      </c>
-      <c r="L27" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L27" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E27,Trigger)</f>
-        <v>42144</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.2">
@@ -3751,13 +3757,13 @@
       <c r="J28" s="12">
         <v>1</v>
       </c>
-      <c r="K28" s="11">
+      <c r="K28" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E28,Trigger)</f>
-        <v>41995</v>
-      </c>
-      <c r="L28" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L28" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E28,Trigger)</f>
-        <v>42177</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.2">
@@ -3827,13 +3833,13 @@
       <c r="J30" s="12">
         <v>1</v>
       </c>
-      <c r="K30" s="11">
+      <c r="K30" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E30,Trigger)</f>
-        <v>42055</v>
-      </c>
-      <c r="L30" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L30" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E30,Trigger)</f>
-        <v>42236</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.2">
@@ -3865,13 +3871,13 @@
       <c r="J31" s="12">
         <v>1</v>
       </c>
-      <c r="K31" s="11">
+      <c r="K31" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E31,Trigger)</f>
-        <v>42083</v>
-      </c>
-      <c r="L31" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L31" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E31,Trigger)</f>
-        <v>42268</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.2">
@@ -3903,13 +3909,13 @@
       <c r="J32" s="12">
         <v>1</v>
       </c>
-      <c r="K32" s="11">
+      <c r="K32" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E32,Trigger)</f>
-        <v>42114</v>
-      </c>
-      <c r="L32" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L32" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E32,Trigger)</f>
-        <v>42297</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -3941,13 +3947,13 @@
       <c r="J33" s="12">
         <v>1</v>
       </c>
-      <c r="K33" s="11">
+      <c r="K33" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E33,Trigger)</f>
-        <v>42144</v>
-      </c>
-      <c r="L33" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L33" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E33,Trigger)</f>
-        <v>42328</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -3979,13 +3985,13 @@
       <c r="J34" s="12">
         <v>1</v>
       </c>
-      <c r="K34" s="11">
+      <c r="K34" s="11" t="e">
         <f>_xll.qlRateHelperEarliestDate($E34,Trigger)</f>
-        <v>42177</v>
-      </c>
-      <c r="L34" s="10">
+        <v>#NUM!</v>
+      </c>
+      <c r="L34" s="10" t="e">
         <f>_xll.qlRateHelperLatestDate($E34,Trigger)</f>
-        <v>42360</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
@@ -9771,10 +9777,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="201" t="s">
+      <c r="A1" s="202" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="202"/>
+      <c r="B1" s="203"/>
       <c r="D1" s="51" t="s">
         <v>83</v>
       </c>
@@ -9978,7 +9984,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_RateHelpersSelected#0003</v>
+        <v>USD_YC6MRH_RateHelpersSelected#0002</v>
       </c>
       <c r="B7" s="41" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10137,9 +10143,9 @@
       <c r="D12" s="40" t="str">
         <v>USD_YC6MRH_1x7F</v>
       </c>
-      <c r="E12" s="39" t="e">
+      <c r="E12" s="39">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>#NUM!</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="F12" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -10167,9 +10173,9 @@
       <c r="D13" s="40" t="str">
         <v>USD_YC6MRH_3x9F</v>
       </c>
-      <c r="E13" s="39" t="e">
+      <c r="E13" s="39">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>#NUM!</v>
+        <v>3.9000000000000003E-3</v>
       </c>
       <c r="F13" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10197,9 +10203,9 @@
       <c r="D14" s="40" t="str">
         <v>USD_YC6MRH_6x12F</v>
       </c>
-      <c r="E14" s="39" t="e">
+      <c r="E14" s="39">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>#NUM!</v>
+        <v>4.3800000000000002E-3</v>
       </c>
       <c r="F14" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -13105,7 +13111,7 @@
       </c>
       <c r="F3" s="101" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_SND#0005</v>
+        <v>USD_YC6MRH_SND#0002</v>
       </c>
       <c r="G3" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13132,7 +13138,7 @@
       </c>
       <c r="F4" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_SWD#0005</v>
+        <v>USD_YC6MRH_SWD#0002</v>
       </c>
       <c r="G4" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13159,7 +13165,7 @@
       </c>
       <c r="F5" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2WD#0005</v>
+        <v>USD_YC6MRH_2WD#0002</v>
       </c>
       <c r="G5" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13186,7 +13192,7 @@
       </c>
       <c r="F6" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3WD#0005</v>
+        <v>USD_YC6MRH_3WD#0002</v>
       </c>
       <c r="G6" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13213,7 +13219,7 @@
       </c>
       <c r="F7" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_1MD#0005</v>
+        <v>USD_YC6MRH_1MD#0002</v>
       </c>
       <c r="G7" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13240,7 +13246,7 @@
       </c>
       <c r="F8" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2MD#0005</v>
+        <v>USD_YC6MRH_2MD#0002</v>
       </c>
       <c r="G8" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13267,7 +13273,7 @@
       </c>
       <c r="F9" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3MD#0005</v>
+        <v>USD_YC6MRH_3MD#0002</v>
       </c>
       <c r="G9" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13294,7 +13300,7 @@
       </c>
       <c r="F10" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_4MD#0005</v>
+        <v>USD_YC6MRH_4MD#0002</v>
       </c>
       <c r="G10" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -13321,7 +13327,7 @@
       </c>
       <c r="F11" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_5MD#0005</v>
+        <v>USD_YC6MRH_5MD#0002</v>
       </c>
       <c r="G11" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -13348,7 +13354,7 @@
       </c>
       <c r="F12" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_6MD#0005</v>
+        <v>USD_YC6MRH_6MD#0002</v>
       </c>
       <c r="G12" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -13435,13 +13441,13 @@
         <f>$H$1&amp;"_FRAs.xml"</f>
         <v>USD_YC6MRH_FRAs.xml</v>
       </c>
-      <c r="I2" s="148">
+      <c r="I2" s="148" t="e">
         <f ca="1">IF(Serialize,_xll.ohObjectSave(I3:I22,SerializationPath&amp;H2,FileOverwrite,Serialize),"---")</f>
-        <v>20</v>
+        <v>#NUM!</v>
       </c>
       <c r="J2" s="147" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I2)</f>
-        <v/>
+        <v>ohObjectSave - operToVectorImpl: error converting parameter 'ObjectList' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'class s</v>
       </c>
       <c r="K2" s="93"/>
     </row>
@@ -13472,13 +13478,13 @@
         <f t="shared" ref="H3:H22" si="2">$H$1&amp;"_"&amp;$C3&amp;$D3</f>
         <v>USD_YC6MRH_T6F1</v>
       </c>
-      <c r="I3" s="139" t="str">
+      <c r="I3" s="139" t="e">
         <f>_xll.qlFraRateHelper(H3,G3,B3,E3,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_T6F1#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J3" s="147" t="str">
-        <f>_xll.ohRangeRetrieveError(I3)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I3)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USDT6F1_Quote'</v>
       </c>
       <c r="K3" s="93"/>
     </row>
@@ -13509,13 +13515,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_TOM6F1</v>
       </c>
-      <c r="I4" s="144" t="str">
+      <c r="I4" s="144" t="e">
         <f>_xll.qlFraRateHelper(H4,G4,B4,E4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_TOM6F1#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J4" s="143" t="str">
-        <f>_xll.ohRangeRetrieveError(I4)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I4)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USDTOM6F1_Quote'</v>
       </c>
       <c r="K4" s="93"/>
     </row>
@@ -13549,7 +13555,7 @@
       </c>
       <c r="I5" s="139" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_1x7F#0005</v>
+        <v>USD_YC6MRH_1x7F#0002</v>
       </c>
       <c r="J5" s="138" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13587,7 +13593,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2x8F#0005</v>
+        <v>USD_YC6MRH_2x8F#0002</v>
       </c>
       <c r="J6" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13625,7 +13631,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3x9F#0005</v>
+        <v>USD_YC6MRH_3x9F#0002</v>
       </c>
       <c r="J7" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13663,7 +13669,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_4x10F#0005</v>
+        <v>USD_YC6MRH_4x10F#0002</v>
       </c>
       <c r="J8" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13701,7 +13707,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_5x11F#0005</v>
+        <v>USD_YC6MRH_5x11F#0002</v>
       </c>
       <c r="J9" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13739,7 +13745,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_6x12F#0005</v>
+        <v>USD_YC6MRH_6x12F#0002</v>
       </c>
       <c r="J10" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -13775,13 +13781,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_7x13F</v>
       </c>
-      <c r="I11" s="134" t="str">
+      <c r="I11" s="134" t="e">
         <f>_xll.qlFraRateHelper(H11,G11,B11,E11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_7x13F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J11" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I11)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I11)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD7x13F_Quote'</v>
       </c>
       <c r="K11" s="93"/>
     </row>
@@ -13813,13 +13819,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_8x14F</v>
       </c>
-      <c r="I12" s="134" t="str">
+      <c r="I12" s="134" t="e">
         <f>_xll.qlFraRateHelper(H12,G12,B12,E12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_8x14F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J12" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I12)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I12)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD8x14F_Quote'</v>
       </c>
       <c r="K12" s="93"/>
     </row>
@@ -13851,13 +13857,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_9x15F</v>
       </c>
-      <c r="I13" s="134" t="str">
+      <c r="I13" s="134" t="e">
         <f>_xll.qlFraRateHelper(H13,G13,B13,E13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_9x15F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J13" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I13)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I13)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD9x15F_Quote'</v>
       </c>
       <c r="K13" s="93"/>
     </row>
@@ -13889,13 +13895,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_10x16F</v>
       </c>
-      <c r="I14" s="134" t="str">
+      <c r="I14" s="134" t="e">
         <f>_xll.qlFraRateHelper(H14,G14,B14,E14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_10x16F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J14" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I14)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I14)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD10x16F_Quote'</v>
       </c>
       <c r="K14" s="93"/>
     </row>
@@ -13927,13 +13933,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_11x17F</v>
       </c>
-      <c r="I15" s="134" t="str">
+      <c r="I15" s="134" t="e">
         <f>_xll.qlFraRateHelper(H15,G15,B15,E15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_11x17F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J15" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I15)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I15)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD11x17F_Quote'</v>
       </c>
       <c r="K15" s="93"/>
     </row>
@@ -13967,7 +13973,7 @@
       </c>
       <c r="I16" s="134" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_12x18F#0005</v>
+        <v>USD_YC6MRH_12x18F#0002</v>
       </c>
       <c r="J16" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14003,13 +14009,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_13x19F</v>
       </c>
-      <c r="I17" s="134" t="str">
+      <c r="I17" s="134" t="e">
         <f>_xll.qlFraRateHelper(H17,G17,B17,E17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_13x19F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J17" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I17)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I17)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD13x19F_Quote'</v>
       </c>
       <c r="K17" s="93"/>
     </row>
@@ -14041,13 +14047,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_14x20F</v>
       </c>
-      <c r="I18" s="134" t="str">
+      <c r="I18" s="134" t="e">
         <f>_xll.qlFraRateHelper(H18,G18,B18,E18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_14x20F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J18" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I18)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I18)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD14x20F_Quote'</v>
       </c>
       <c r="K18" s="93"/>
     </row>
@@ -14079,13 +14085,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_15x21F</v>
       </c>
-      <c r="I19" s="134" t="str">
+      <c r="I19" s="134" t="e">
         <f>_xll.qlFraRateHelper(H19,G19,B19,E19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_15x21F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J19" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I19)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I19)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD15x21F_Quote'</v>
       </c>
       <c r="K19" s="93"/>
     </row>
@@ -14117,13 +14123,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_16x22F</v>
       </c>
-      <c r="I20" s="134" t="str">
+      <c r="I20" s="134" t="e">
         <f>_xll.qlFraRateHelper(H20,G20,B20,E20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_16x22F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J20" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I20)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I20)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD16x22F_Quote'</v>
       </c>
       <c r="K20" s="93"/>
     </row>
@@ -14155,13 +14161,13 @@
         <f t="shared" si="2"/>
         <v>USD_YC6MRH_17x23F</v>
       </c>
-      <c r="I21" s="134" t="str">
+      <c r="I21" s="134" t="e">
         <f>_xll.qlFraRateHelper(H21,G21,B21,E21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_17x23F#0005</v>
+        <v>#NUM!</v>
       </c>
       <c r="J21" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I21)</f>
-        <v/>
+        <f ca="1">_xll.ohRangeRetrieveError(I21)</f>
+        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD17x23F_Quote'</v>
       </c>
       <c r="K21" s="93"/>
     </row>
@@ -14195,7 +14201,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_18x24F#0005</v>
+        <v>USD_YC6MRH_18x24F#0002</v>
       </c>
       <c r="J22" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14232,9 +14238,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:AB43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14245,11 +14253,11 @@
     <col min="5" max="5" width="2.7109375" style="108" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.85546875" style="108" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="108" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="108" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="108" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.140625" style="108" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" style="108" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27.5703125" style="108" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" style="130" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.5703125" style="108" customWidth="1"/>
     <col min="14" max="14" width="3.85546875" style="108" customWidth="1"/>
     <col min="15" max="15" width="2.5703125" style="108" customWidth="1"/>
@@ -14259,7 +14267,7 @@
     <col min="19" max="16384" width="9.140625" style="108"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="185" t="s">
         <v>188</v>
       </c>
@@ -14277,7 +14285,7 @@
       <c r="M1" s="159"/>
       <c r="N1" s="184"/>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="100"/>
       <c r="B2" s="110"/>
       <c r="C2" s="110"/>
@@ -14303,7 +14311,7 @@
       <c r="M2" s="110"/>
       <c r="N2" s="162"/>
     </row>
-    <row r="3" spans="1:28" ht="22.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A3" s="100"/>
       <c r="B3" s="107" t="s">
         <v>178</v>
@@ -14340,7 +14348,7 @@
       </c>
       <c r="N3" s="162"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="111"/>
       <c r="B4" s="110"/>
       <c r="C4" s="110"/>
@@ -14357,7 +14365,7 @@
       </c>
       <c r="L4" s="180" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>USD_YC6MRH_AM6LBASIS_Libor6M#0005</v>
+        <v>USD_YC6MRH_AM6LBASIS_Libor6M#0002</v>
       </c>
       <c r="M4" s="179" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -14365,7 +14373,7 @@
       </c>
       <c r="N4" s="162"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="111"/>
       <c r="B5" s="110"/>
       <c r="C5" s="110"/>
@@ -14381,7 +14389,7 @@
       <c r="M5" s="110"/>
       <c r="N5" s="162"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="100"/>
       <c r="B6" s="178" t="s">
         <v>169</v>
@@ -14421,7 +14429,7 @@
       </c>
       <c r="L6" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS1Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS1Y#0002</v>
       </c>
       <c r="M6" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -14429,7 +14437,7 @@
       </c>
       <c r="N6" s="162"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="100"/>
       <c r="B7" s="168" t="str">
         <f t="shared" ref="B7:B42" si="4">B6</f>
@@ -14475,7 +14483,7 @@
       </c>
       <c r="N7" s="162"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="100"/>
       <c r="B8" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14521,7 +14529,7 @@
       </c>
       <c r="N8" s="162"/>
     </row>
-    <row r="9" spans="1:28" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="100"/>
       <c r="B9" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14567,7 +14575,7 @@
       </c>
       <c r="N9" s="162"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="100"/>
       <c r="B10" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14608,7 +14616,7 @@
       </c>
       <c r="L10" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS2Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS2Y#0002</v>
       </c>
       <c r="M10" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -14624,12 +14632,12 @@
       <c r="R10" s="175" t="s">
         <v>172</v>
       </c>
-      <c r="AB10" s="108" t="str">
-        <f>_xll.ohObjectCallerAddress(J10)</f>
-        <v>'[USD_Market.xlsm]6M (2)'!R4C11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T10" s="108" t="e">
+        <f>_xll.qlQuoteValue(J10)</f>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="100"/>
       <c r="B11" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14670,7 +14678,7 @@
       </c>
       <c r="L11" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS3Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS3Y#0002</v>
       </c>
       <c r="M11" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -14687,7 +14695,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="100"/>
       <c r="B12" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14728,7 +14736,7 @@
       </c>
       <c r="L12" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS4Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS4Y#0002</v>
       </c>
       <c r="M12" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -14745,7 +14753,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="100"/>
       <c r="B13" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14786,7 +14794,7 @@
       </c>
       <c r="L13" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS5Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS5Y#0002</v>
       </c>
       <c r="M13" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -14803,7 +14811,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="100"/>
       <c r="B14" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14844,7 +14852,7 @@
       </c>
       <c r="L14" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS6Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS6Y#0002</v>
       </c>
       <c r="M14" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -14861,7 +14869,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="100"/>
       <c r="B15" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14902,7 +14910,7 @@
       </c>
       <c r="L15" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS7Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS7Y#0002</v>
       </c>
       <c r="M15" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -14913,7 +14921,7 @@
       <c r="Q15" s="169"/>
       <c r="R15" s="169"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="100"/>
       <c r="B16" s="168" t="str">
         <f t="shared" si="4"/>
@@ -14954,7 +14962,7 @@
       </c>
       <c r="L16" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS8Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS8Y#0002</v>
       </c>
       <c r="M16" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -15003,7 +15011,7 @@
       </c>
       <c r="L17" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS9Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS9Y#0002</v>
       </c>
       <c r="M17" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -15052,7 +15060,7 @@
       </c>
       <c r="L18" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS10Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS10Y#0002</v>
       </c>
       <c r="M18" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -15101,7 +15109,7 @@
       </c>
       <c r="L19" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS11Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS11Y#0002</v>
       </c>
       <c r="M19" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -15150,7 +15158,7 @@
       </c>
       <c r="L20" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS12Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS12Y#0002</v>
       </c>
       <c r="M20" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -15199,7 +15207,7 @@
       </c>
       <c r="L21" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS13Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS13Y#0002</v>
       </c>
       <c r="M21" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -15248,7 +15256,7 @@
       </c>
       <c r="L22" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS14Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS14Y#0002</v>
       </c>
       <c r="M22" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -15297,7 +15305,7 @@
       </c>
       <c r="L23" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS15Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS15Y#0002</v>
       </c>
       <c r="M23" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -15346,7 +15354,7 @@
       </c>
       <c r="L24" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS16Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS16Y#0002</v>
       </c>
       <c r="M24" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -15395,7 +15403,7 @@
       </c>
       <c r="L25" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS17Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS17Y#0002</v>
       </c>
       <c r="M25" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -15444,7 +15452,7 @@
       </c>
       <c r="L26" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS18Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS18Y#0002</v>
       </c>
       <c r="M26" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -15493,7 +15501,7 @@
       </c>
       <c r="L27" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS19Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS19Y#0002</v>
       </c>
       <c r="M27" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -15542,7 +15550,7 @@
       </c>
       <c r="L28" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS20Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS20Y#0002</v>
       </c>
       <c r="M28" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -15591,7 +15599,7 @@
       </c>
       <c r="L29" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS21Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS21Y#0002</v>
       </c>
       <c r="M29" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -15640,7 +15648,7 @@
       </c>
       <c r="L30" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS22Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS22Y#0002</v>
       </c>
       <c r="M30" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -15689,7 +15697,7 @@
       </c>
       <c r="L31" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS23Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS23Y#0002</v>
       </c>
       <c r="M31" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -15738,7 +15746,7 @@
       </c>
       <c r="L32" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS24Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS24Y#0002</v>
       </c>
       <c r="M32" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -15787,7 +15795,7 @@
       </c>
       <c r="L33" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS25Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS25Y#0002</v>
       </c>
       <c r="M33" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -15836,7 +15844,7 @@
       </c>
       <c r="L34" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS26Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS26Y#0002</v>
       </c>
       <c r="M34" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -15885,7 +15893,7 @@
       </c>
       <c r="L35" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS27Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS27Y#0002</v>
       </c>
       <c r="M35" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -15934,7 +15942,7 @@
       </c>
       <c r="L36" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS28Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS28Y#0002</v>
       </c>
       <c r="M36" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -15983,7 +15991,7 @@
       </c>
       <c r="L37" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS29Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS29Y#0002</v>
       </c>
       <c r="M37" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -16032,7 +16040,7 @@
       </c>
       <c r="L38" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS30Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS30Y#0002</v>
       </c>
       <c r="M38" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -16081,7 +16089,7 @@
       </c>
       <c r="L39" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS35Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS35Y#0002</v>
       </c>
       <c r="M39" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -16130,7 +16138,7 @@
       </c>
       <c r="L40" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS40Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS40Y#0002</v>
       </c>
       <c r="M40" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -16179,7 +16187,7 @@
       </c>
       <c r="L41" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS50Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS50Y#0002</v>
       </c>
       <c r="M41" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -16228,7 +16236,7 @@
       </c>
       <c r="L42" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS60Y#0003</v>
+        <v>USD_YC6MRH_AM6LBASIS60Y#0002</v>
       </c>
       <c r="M42" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>

<commit_message>
enable Live Data Toggle button
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/USD_YC6MBootstrapping.xlsx
+++ b/QuantLibXL/Data2/XLS/USD_YC6MBootstrapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="24540" windowHeight="7620" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="24540" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="6" r:id="rId1"/>
@@ -2191,7 +2191,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:N30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2211,7 +2211,7 @@
     <row r="1" spans="2:14" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="186" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Jan 15 2014 16:53:36</v>
+        <v>QuantLibXL 1.3.0 - MS VC++ 9.0 - Multithreaded Static Runtime library - Release Configuration - Dec  5 2013 11:03:51</v>
       </c>
     </row>
     <row r="2" spans="2:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2285,7 +2285,7 @@
       </c>
       <c r="M5" s="127" t="str">
         <f ca="1">SUBSTITUTE(LEFT(CELL("filename",A1),FIND("[",CELL("filename",A1),1)-1),"\XLS\","\XML\")</f>
-        <v>C:\erik\repos\quantlib\QuantLibXL\Data2\XML\</v>
+        <v>C:\Users\erik\Documents\repos\quantlib_nando\QuantLibXL\Data2\XML\</v>
       </c>
       <c r="N5" s="124"/>
     </row>
@@ -2396,7 +2396,7 @@
         <v>100</v>
       </c>
       <c r="D11" s="84">
-        <v>41655.710428240738</v>
+        <v>41666.693993055553</v>
       </c>
       <c r="E11" s="56"/>
       <c r="F11" s="55"/>
@@ -2450,7 +2450,7 @@
       </c>
       <c r="D14" s="81" t="str">
         <f>_xll.qlPiecewiseYieldCurve(D16,NDays,Calendar,RateHelpersSelected,DayCounter,IF(ISERROR(D22),NA(),D20:E20),IF(ISERROR(D22),NA(),D21:E21),Accuracy,TraitsID,InterpolatorID,Permanent,,ObjectOverwrite)</f>
-        <v>_USDYC6M#0002</v>
+        <v>_USDYC6M#0000</v>
       </c>
       <c r="E14" s="56"/>
       <c r="F14" s="55"/>
@@ -2629,7 +2629,7 @@
       <c r="B27" s="59"/>
       <c r="C27" s="63">
         <f>_xll.qlTermStructureReferenceDate(YieldCurve)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="D27" s="62" t="e">
         <f>MAX(_xll.ohPack(Selected!I1:I126))</f>
@@ -2658,7 +2658,7 @@
       </c>
       <c r="D29" s="57" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(Selected!I1)</f>
-        <v>qlPiecewiseYieldCurveData - 14th instrument (maturity: January 20th, 2016) has an invalid quote</v>
+        <v>qlPiecewiseYieldCurveData - 14th instrument (maturity: January 21st, 2016) has an invalid quote</v>
       </c>
       <c r="E29" s="56"/>
       <c r="F29" s="55"/>
@@ -2872,11 +2872,11 @@
       </c>
       <c r="K4" s="11">
         <f>_xll.qlRateHelperEarliestDate($E4,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L4" s="10">
         <f>_xll.qlRateHelperLatestDate($E4,Trigger)</f>
-        <v>41660</v>
+        <v>41661</v>
       </c>
       <c r="M4" s="1">
         <v>30</v>
@@ -2911,11 +2911,11 @@
       </c>
       <c r="K5" s="11">
         <f>_xll.qlRateHelperEarliestDate($E5,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L5" s="10">
         <f>_xll.qlRateHelperLatestDate($E5,Trigger)</f>
-        <v>41666</v>
+        <v>41667</v>
       </c>
       <c r="M5" s="1">
         <v>40</v>
@@ -2950,11 +2950,11 @@
       </c>
       <c r="K6" s="11">
         <f>_xll.qlRateHelperEarliestDate($E6,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L6" s="10">
         <f>_xll.qlRateHelperLatestDate($E6,Trigger)</f>
-        <v>41673</v>
+        <v>41674</v>
       </c>
       <c r="M6" s="1">
         <v>50</v>
@@ -2989,11 +2989,11 @@
       </c>
       <c r="K7" s="11">
         <f>_xll.qlRateHelperEarliestDate($E7,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L7" s="10">
         <f>_xll.qlRateHelperLatestDate($E7,Trigger)</f>
-        <v>41680</v>
+        <v>41681</v>
       </c>
       <c r="M7" s="1">
         <v>60</v>
@@ -3028,11 +3028,11 @@
       </c>
       <c r="K8" s="11">
         <f>_xll.qlRateHelperEarliestDate($E8,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L8" s="10">
         <f>_xll.qlRateHelperLatestDate($E8,Trigger)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="M8" s="1">
         <v>70</v>
@@ -3067,11 +3067,11 @@
       </c>
       <c r="K9" s="11">
         <f>_xll.qlRateHelperEarliestDate($E9,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L9" s="10">
         <f>_xll.qlRateHelperLatestDate($E9,Trigger)</f>
-        <v>41718</v>
+        <v>41719</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="K10" s="11">
         <f>_xll.qlRateHelperEarliestDate($E10,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L10" s="10">
         <f>_xll.qlRateHelperLatestDate($E10,Trigger)</f>
@@ -3133,11 +3133,11 @@
       </c>
       <c r="K11" s="11">
         <f>_xll.qlRateHelperEarliestDate($E11,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L11" s="10">
         <f>_xll.qlRateHelperLatestDate($E11,Trigger)</f>
-        <v>41779</v>
+        <v>41780</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -3166,11 +3166,11 @@
       </c>
       <c r="K12" s="11">
         <f>_xll.qlRateHelperEarliestDate($E12,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L12" s="10">
         <f>_xll.qlRateHelperLatestDate($E12,Trigger)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -3199,7 +3199,7 @@
       </c>
       <c r="K13" s="11">
         <f>_xll.qlRateHelperEarliestDate($E13,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L13" s="10">
         <f>_xll.qlRateHelperLatestDate($E13,Trigger)</f>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="F18" s="13">
         <f>_xll.qlRateHelperQuoteValue($E18,Trigger)</f>
-        <v>3.5999999999999999E-3</v>
+        <v>3.4699999999999996E-3</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="12" t="b">
@@ -3379,11 +3379,11 @@
       </c>
       <c r="K18" s="11">
         <f>_xll.qlRateHelperEarliestDate($E18,Trigger)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="L18" s="10">
         <f>_xll.qlRateHelperLatestDate($E18,Trigger)</f>
-        <v>41871</v>
+        <v>41872</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
@@ -3403,7 +3403,7 @@
       </c>
       <c r="F19" s="13">
         <f>_xll.qlRateHelperQuoteValue($E19,Trigger)</f>
-        <v>3.7599999999999999E-3</v>
+        <v>3.5899999999999999E-3</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="12" t="b">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="K19" s="11">
         <f>_xll.qlRateHelperEarliestDate($E19,Trigger)</f>
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="L19" s="10">
         <f>_xll.qlRateHelperLatestDate($E19,Trigger)</f>
@@ -3441,7 +3441,7 @@
       </c>
       <c r="F20" s="13">
         <f>_xll.qlRateHelperQuoteValue($E20,Trigger)</f>
-        <v>3.9000000000000003E-3</v>
+        <v>3.79E-3</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="12" t="b">
@@ -3479,7 +3479,7 @@
       </c>
       <c r="F21" s="13">
         <f>_xll.qlRateHelperQuoteValue($E21,Trigger)</f>
-        <v>4.0400000000000002E-3</v>
+        <v>3.96E-3</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="12" t="b">
@@ -3493,11 +3493,11 @@
       </c>
       <c r="K21" s="11">
         <f>_xll.qlRateHelperEarliestDate($E21,Trigger)</f>
-        <v>41779</v>
+        <v>41780</v>
       </c>
       <c r="L21" s="10">
         <f>_xll.qlRateHelperLatestDate($E21,Trigger)</f>
-        <v>41963</v>
+        <v>41964</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
@@ -3517,7 +3517,7 @@
       </c>
       <c r="F22" s="13">
         <f>_xll.qlRateHelperQuoteValue($E22,Trigger)</f>
-        <v>4.2000000000000006E-3</v>
+        <v>4.13E-3</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="12" t="b">
@@ -3531,11 +3531,11 @@
       </c>
       <c r="K22" s="11">
         <f>_xll.qlRateHelperEarliestDate($E22,Trigger)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="L22" s="10">
         <f>_xll.qlRateHelperLatestDate($E22,Trigger)</f>
-        <v>41995</v>
+        <v>41996</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
@@ -3555,7 +3555,7 @@
       </c>
       <c r="F23" s="13">
         <f>_xll.qlRateHelperQuoteValue($E23,Trigger)</f>
-        <v>4.3800000000000002E-3</v>
+        <v>4.3899999999999998E-3</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="12" t="b">
@@ -3797,11 +3797,11 @@
       </c>
       <c r="K29" s="11">
         <f>_xll.qlRateHelperEarliestDate($E29,Trigger)</f>
-        <v>42024</v>
+        <v>42025</v>
       </c>
       <c r="L29" s="10">
         <f>_xll.qlRateHelperLatestDate($E29,Trigger)</f>
-        <v>42205</v>
+        <v>42206</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.2">
@@ -4025,11 +4025,11 @@
       </c>
       <c r="K35" s="4">
         <f>_xll.qlRateHelperEarliestDate($E35,Trigger)</f>
-        <v>42205</v>
+        <v>42206</v>
       </c>
       <c r="L35" s="3">
         <f>_xll.qlRateHelperLatestDate($E35,Trigger)</f>
-        <v>42389</v>
+        <v>42390</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -8221,11 +8221,11 @@
       </c>
       <c r="K133" s="11">
         <f>_xll.qlRateHelperEarliestDate($E133,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L133" s="10">
         <f>_xll.qlRateHelperLatestDate($E133,Trigger)</f>
-        <v>42024</v>
+        <v>42025</v>
       </c>
     </row>
     <row r="134" spans="2:14" x14ac:dyDescent="0.2">
@@ -8389,11 +8389,11 @@
       </c>
       <c r="K137" s="11">
         <f>_xll.qlRateHelperEarliestDate($E137,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L137" s="10">
         <f>_xll.qlRateHelperLatestDate($E137,Trigger)</f>
-        <v>42389</v>
+        <v>42390</v>
       </c>
     </row>
     <row r="138" spans="2:14" x14ac:dyDescent="0.2">
@@ -8431,11 +8431,11 @@
       </c>
       <c r="K138" s="11">
         <f>_xll.qlRateHelperEarliestDate($E138,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L138" s="10">
         <f>_xll.qlRateHelperLatestDate($E138,Trigger)</f>
-        <v>42755</v>
+        <v>42758</v>
       </c>
     </row>
     <row r="139" spans="2:14" x14ac:dyDescent="0.2">
@@ -8473,7 +8473,7 @@
       </c>
       <c r="K139" s="11">
         <f>_xll.qlRateHelperEarliestDate($E139,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L139" s="10">
         <f>_xll.qlRateHelperLatestDate($E139,Trigger)</f>
@@ -8515,7 +8515,7 @@
       </c>
       <c r="K140" s="11">
         <f>_xll.qlRateHelperEarliestDate($E140,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L140" s="10">
         <f>_xll.qlRateHelperLatestDate($E140,Trigger)</f>
@@ -8557,11 +8557,11 @@
       </c>
       <c r="K141" s="11">
         <f>_xll.qlRateHelperEarliestDate($E141,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L141" s="10">
         <f>_xll.qlRateHelperLatestDate($E141,Trigger)</f>
-        <v>43850</v>
+        <v>43851</v>
       </c>
     </row>
     <row r="142" spans="2:14" x14ac:dyDescent="0.2">
@@ -8599,11 +8599,11 @@
       </c>
       <c r="K142" s="11">
         <f>_xll.qlRateHelperEarliestDate($E142,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L142" s="10">
         <f>_xll.qlRateHelperLatestDate($E142,Trigger)</f>
-        <v>44216</v>
+        <v>44217</v>
       </c>
     </row>
     <row r="143" spans="2:14" x14ac:dyDescent="0.2">
@@ -8641,11 +8641,11 @@
       </c>
       <c r="K143" s="11">
         <f>_xll.qlRateHelperEarliestDate($E143,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L143" s="10">
         <f>_xll.qlRateHelperLatestDate($E143,Trigger)</f>
-        <v>44581</v>
+        <v>44582</v>
       </c>
     </row>
     <row r="144" spans="2:14" x14ac:dyDescent="0.2">
@@ -8683,11 +8683,11 @@
       </c>
       <c r="K144" s="11">
         <f>_xll.qlRateHelperEarliestDate($E144,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L144" s="10">
         <f>_xll.qlRateHelperLatestDate($E144,Trigger)</f>
-        <v>44946</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="145" spans="2:12" x14ac:dyDescent="0.2">
@@ -8725,7 +8725,7 @@
       </c>
       <c r="K145" s="11">
         <f>_xll.qlRateHelperEarliestDate($E145,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L145" s="10">
         <f>_xll.qlRateHelperLatestDate($E145,Trigger)</f>
@@ -8767,11 +8767,11 @@
       </c>
       <c r="K146" s="11">
         <f>_xll.qlRateHelperEarliestDate($E146,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L146" s="10">
         <f>_xll.qlRateHelperLatestDate($E146,Trigger)</f>
-        <v>45677</v>
+        <v>45678</v>
       </c>
     </row>
     <row r="147" spans="2:12" x14ac:dyDescent="0.2">
@@ -8809,11 +8809,11 @@
       </c>
       <c r="K147" s="11">
         <f>_xll.qlRateHelperEarliestDate($E147,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L147" s="10">
         <f>_xll.qlRateHelperLatestDate($E147,Trigger)</f>
-        <v>46042</v>
+        <v>46043</v>
       </c>
     </row>
     <row r="148" spans="2:12" x14ac:dyDescent="0.2">
@@ -8851,11 +8851,11 @@
       </c>
       <c r="K148" s="11">
         <f>_xll.qlRateHelperEarliestDate($E148,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L148" s="10">
         <f>_xll.qlRateHelperLatestDate($E148,Trigger)</f>
-        <v>46407</v>
+        <v>46408</v>
       </c>
     </row>
     <row r="149" spans="2:12" x14ac:dyDescent="0.2">
@@ -8893,11 +8893,11 @@
       </c>
       <c r="K149" s="11">
         <f>_xll.qlRateHelperEarliestDate($E149,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L149" s="10">
         <f>_xll.qlRateHelperLatestDate($E149,Trigger)</f>
-        <v>46772</v>
+        <v>46773</v>
       </c>
     </row>
     <row r="150" spans="2:12" x14ac:dyDescent="0.2">
@@ -8935,7 +8935,7 @@
       </c>
       <c r="K150" s="11">
         <f>_xll.qlRateHelperEarliestDate($E150,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L150" s="10">
         <f>_xll.qlRateHelperLatestDate($E150,Trigger)</f>
@@ -8977,7 +8977,7 @@
       </c>
       <c r="K151" s="11">
         <f>_xll.qlRateHelperEarliestDate($E151,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L151" s="10">
         <f>_xll.qlRateHelperLatestDate($E151,Trigger)</f>
@@ -9019,11 +9019,11 @@
       </c>
       <c r="K152" s="11">
         <f>_xll.qlRateHelperEarliestDate($E152,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L152" s="10">
         <f>_xll.qlRateHelperLatestDate($E152,Trigger)</f>
-        <v>47868</v>
+        <v>47869</v>
       </c>
     </row>
     <row r="153" spans="2:12" x14ac:dyDescent="0.2">
@@ -9061,11 +9061,11 @@
       </c>
       <c r="K153" s="11">
         <f>_xll.qlRateHelperEarliestDate($E153,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L153" s="10">
         <f>_xll.qlRateHelperLatestDate($E153,Trigger)</f>
-        <v>48233</v>
+        <v>48234</v>
       </c>
     </row>
     <row r="154" spans="2:12" x14ac:dyDescent="0.2">
@@ -9103,11 +9103,11 @@
       </c>
       <c r="K154" s="11">
         <f>_xll.qlRateHelperEarliestDate($E154,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L154" s="10">
         <f>_xll.qlRateHelperLatestDate($E154,Trigger)</f>
-        <v>48599</v>
+        <v>48600</v>
       </c>
     </row>
     <row r="155" spans="2:12" x14ac:dyDescent="0.2">
@@ -9145,11 +9145,11 @@
       </c>
       <c r="K155" s="11">
         <f>_xll.qlRateHelperEarliestDate($E155,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L155" s="10">
         <f>_xll.qlRateHelperLatestDate($E155,Trigger)</f>
-        <v>48964</v>
+        <v>48967</v>
       </c>
     </row>
     <row r="156" spans="2:12" x14ac:dyDescent="0.2">
@@ -9187,7 +9187,7 @@
       </c>
       <c r="K156" s="11">
         <f>_xll.qlRateHelperEarliestDate($E156,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L156" s="10">
         <f>_xll.qlRateHelperLatestDate($E156,Trigger)</f>
@@ -9229,7 +9229,7 @@
       </c>
       <c r="K157" s="11">
         <f>_xll.qlRateHelperEarliestDate($E157,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L157" s="10">
         <f>_xll.qlRateHelperLatestDate($E157,Trigger)</f>
@@ -9271,11 +9271,11 @@
       </c>
       <c r="K158" s="11">
         <f>_xll.qlRateHelperEarliestDate($E158,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L158" s="10">
         <f>_xll.qlRateHelperLatestDate($E158,Trigger)</f>
-        <v>50060</v>
+        <v>50061</v>
       </c>
     </row>
     <row r="159" spans="2:12" x14ac:dyDescent="0.2">
@@ -9313,11 +9313,11 @@
       </c>
       <c r="K159" s="11">
         <f>_xll.qlRateHelperEarliestDate($E159,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L159" s="10">
         <f>_xll.qlRateHelperLatestDate($E159,Trigger)</f>
-        <v>50425</v>
+        <v>50426</v>
       </c>
     </row>
     <row r="160" spans="2:12" x14ac:dyDescent="0.2">
@@ -9355,11 +9355,11 @@
       </c>
       <c r="K160" s="11">
         <f>_xll.qlRateHelperEarliestDate($E160,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L160" s="10">
         <f>_xll.qlRateHelperLatestDate($E160,Trigger)</f>
-        <v>50790</v>
+        <v>50791</v>
       </c>
     </row>
     <row r="161" spans="2:12" x14ac:dyDescent="0.2">
@@ -9397,11 +9397,11 @@
       </c>
       <c r="K161" s="11">
         <f>_xll.qlRateHelperEarliestDate($E161,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L161" s="10">
         <f>_xll.qlRateHelperLatestDate($E161,Trigger)</f>
-        <v>51155</v>
+        <v>51158</v>
       </c>
     </row>
     <row r="162" spans="2:12" x14ac:dyDescent="0.2">
@@ -9439,7 +9439,7 @@
       </c>
       <c r="K162" s="11">
         <f>_xll.qlRateHelperEarliestDate($E162,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L162" s="10">
         <f>_xll.qlRateHelperLatestDate($E162,Trigger)</f>
@@ -9481,11 +9481,11 @@
       </c>
       <c r="K163" s="11">
         <f>_xll.qlRateHelperEarliestDate($E163,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L163" s="10">
         <f>_xll.qlRateHelperLatestDate($E163,Trigger)</f>
-        <v>51886</v>
+        <v>51887</v>
       </c>
     </row>
     <row r="164" spans="2:12" x14ac:dyDescent="0.2">
@@ -9523,11 +9523,11 @@
       </c>
       <c r="K164" s="11">
         <f>_xll.qlRateHelperEarliestDate($E164,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L164" s="10">
         <f>_xll.qlRateHelperLatestDate($E164,Trigger)</f>
-        <v>52251</v>
+        <v>52252</v>
       </c>
     </row>
     <row r="165" spans="2:12" x14ac:dyDescent="0.2">
@@ -9565,11 +9565,11 @@
       </c>
       <c r="K165" s="11">
         <f>_xll.qlRateHelperEarliestDate($E165,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L165" s="10">
         <f>_xll.qlRateHelperLatestDate($E165,Trigger)</f>
-        <v>52616</v>
+        <v>52617</v>
       </c>
     </row>
     <row r="166" spans="2:12" x14ac:dyDescent="0.2">
@@ -9607,11 +9607,11 @@
       </c>
       <c r="K166" s="11">
         <f>_xll.qlRateHelperEarliestDate($E166,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L166" s="10">
         <f>_xll.qlRateHelperLatestDate($E166,Trigger)</f>
-        <v>54443</v>
+        <v>54444</v>
       </c>
     </row>
     <row r="167" spans="2:12" x14ac:dyDescent="0.2">
@@ -9649,11 +9649,11 @@
       </c>
       <c r="K167" s="11">
         <f>_xll.qlRateHelperEarliestDate($E167,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L167" s="10">
         <f>_xll.qlRateHelperLatestDate($E167,Trigger)</f>
-        <v>56269</v>
+        <v>56270</v>
       </c>
     </row>
     <row r="168" spans="2:12" x14ac:dyDescent="0.2">
@@ -9691,7 +9691,7 @@
       </c>
       <c r="K168" s="11">
         <f>_xll.qlRateHelperEarliestDate($E168,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L168" s="10">
         <f>_xll.qlRateHelperLatestDate($E168,Trigger)</f>
@@ -9733,7 +9733,7 @@
       </c>
       <c r="K169" s="4">
         <f>_xll.qlRateHelperEarliestDate($E169,Trigger)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="L169" s="3">
         <f>_xll.qlRateHelperLatestDate($E169,Trigger)</f>
@@ -9820,11 +9820,11 @@
       </c>
       <c r="G2" s="38">
         <f>_xll.qlRateHelperEarliestDate($D2)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H2" s="37">
         <f>_xll.qlRateHelperLatestDate($D2)</f>
-        <v>41660</v>
+        <v>41661</v>
       </c>
       <c r="I2" s="32" t="e">
         <v>#NUM!</v>
@@ -9856,11 +9856,11 @@
       </c>
       <c r="G3" s="38">
         <f>_xll.qlRateHelperEarliestDate($D3)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H3" s="37">
         <f>_xll.qlRateHelperLatestDate($D3)</f>
-        <v>41666</v>
+        <v>41667</v>
       </c>
       <c r="I3" s="32" t="e">
         <v>#NUM!</v>
@@ -9892,11 +9892,11 @@
       </c>
       <c r="G4" s="38">
         <f>_xll.qlRateHelperEarliestDate($D4)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H4" s="37">
         <f>_xll.qlRateHelperLatestDate($D4)</f>
-        <v>41673</v>
+        <v>41674</v>
       </c>
       <c r="I4" s="32" t="e">
         <v>#NUM!</v>
@@ -9928,11 +9928,11 @@
       </c>
       <c r="G5" s="38">
         <f>_xll.qlRateHelperEarliestDate($D5)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H5" s="37">
         <f>_xll.qlRateHelperLatestDate($D5)</f>
-        <v>41680</v>
+        <v>41681</v>
       </c>
       <c r="I5" s="32" t="e">
         <v>#NUM!</v>
@@ -9965,11 +9965,11 @@
       </c>
       <c r="G6" s="38">
         <f>_xll.qlRateHelperEarliestDate($D6)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H6" s="37">
         <f>_xll.qlRateHelperLatestDate($D6)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="I6" s="32" t="e">
         <v>#NUM!</v>
@@ -9984,7 +9984,7 @@
     <row r="7" spans="1:12" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="str">
         <f>_xll.ohGroup(RateHelperPrefix&amp;"_RateHelpersSelected",_xll.ohPack(Selected!D2:D126),TRUE,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_RateHelpersSelected#0002</v>
+        <v>USD_YC6MRH_RateHelpersSelected#0000</v>
       </c>
       <c r="B7" s="41" t="str">
         <f>_xll.ohRangeRetrieveError(RateHelpersSelected)</f>
@@ -10003,11 +10003,11 @@
       </c>
       <c r="G7" s="38">
         <f>_xll.qlRateHelperEarliestDate($D7)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H7" s="37">
         <f>_xll.qlRateHelperLatestDate($D7)</f>
-        <v>41718</v>
+        <v>41719</v>
       </c>
       <c r="I7" s="32" t="e">
         <v>#NUM!</v>
@@ -10033,7 +10033,7 @@
       </c>
       <c r="G8" s="38">
         <f>_xll.qlRateHelperEarliestDate($D8)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H8" s="37">
         <f>_xll.qlRateHelperLatestDate($D8)</f>
@@ -10063,11 +10063,11 @@
       </c>
       <c r="G9" s="38">
         <f>_xll.qlRateHelperEarliestDate($D9)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H9" s="37">
         <f>_xll.qlRateHelperLatestDate($D9)</f>
-        <v>41779</v>
+        <v>41780</v>
       </c>
       <c r="I9" s="32" t="e">
         <v>#NUM!</v>
@@ -10093,11 +10093,11 @@
       </c>
       <c r="G10" s="38">
         <f>_xll.qlRateHelperEarliestDate($D10)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H10" s="37">
         <f>_xll.qlRateHelperLatestDate($D10)</f>
-        <v>41810</v>
+        <v>41813</v>
       </c>
       <c r="I10" s="32" t="e">
         <v>#NUM!</v>
@@ -10123,7 +10123,7 @@
       </c>
       <c r="G11" s="38">
         <f>_xll.qlRateHelperEarliestDate($D11)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H11" s="37">
         <f>_xll.qlRateHelperLatestDate($D11)</f>
@@ -10145,7 +10145,7 @@
       </c>
       <c r="E12" s="39">
         <f>_xll.qlRateHelperRate($D12)</f>
-        <v>3.5999999999999999E-3</v>
+        <v>3.4699999999999996E-3</v>
       </c>
       <c r="F12" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D12)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D12)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D12)),_xll.qlSwapRateHelperSpread($D12))</f>
@@ -10153,11 +10153,11 @@
       </c>
       <c r="G12" s="38">
         <f>_xll.qlRateHelperEarliestDate($D12)</f>
-        <v>41690</v>
+        <v>41691</v>
       </c>
       <c r="H12" s="37">
         <f>_xll.qlRateHelperLatestDate($D12)</f>
-        <v>41871</v>
+        <v>41872</v>
       </c>
       <c r="I12" s="32" t="e">
         <v>#NUM!</v>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="E13" s="39">
         <f>_xll.qlRateHelperRate($D13)</f>
-        <v>3.9000000000000003E-3</v>
+        <v>3.79E-3</v>
       </c>
       <c r="F13" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D13)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D13)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D13)),_xll.qlSwapRateHelperSpread($D13))</f>
@@ -10205,7 +10205,7 @@
       </c>
       <c r="E14" s="39">
         <f>_xll.qlRateHelperRate($D14)</f>
-        <v>4.3800000000000002E-3</v>
+        <v>4.3899999999999998E-3</v>
       </c>
       <c r="F14" s="39" t="str">
         <f>IF(ISERROR(_xll.qlSwapRateHelperSpread($D14)),IF(ISERROR(_xll.qlFuturesRateHelperConvexityAdjustment($D14)),"--",_xll.qlFuturesRateHelperConvexityAdjustment($D14)),_xll.qlSwapRateHelperSpread($D14))</f>
@@ -10243,11 +10243,11 @@
       </c>
       <c r="G15" s="38">
         <f>_xll.qlRateHelperEarliestDate($D15)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H15" s="37">
         <f>_xll.qlRateHelperLatestDate($D15)</f>
-        <v>42389</v>
+        <v>42390</v>
       </c>
       <c r="I15" s="32" t="e">
         <v>#NUM!</v>
@@ -10273,11 +10273,11 @@
       </c>
       <c r="G16" s="38">
         <f>_xll.qlRateHelperEarliestDate($D16)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H16" s="37">
         <f>_xll.qlRateHelperLatestDate($D16)</f>
-        <v>42755</v>
+        <v>42758</v>
       </c>
       <c r="I16" s="32" t="e">
         <v>#NUM!</v>
@@ -10303,7 +10303,7 @@
       </c>
       <c r="G17" s="38">
         <f>_xll.qlRateHelperEarliestDate($D17)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H17" s="37">
         <f>_xll.qlRateHelperLatestDate($D17)</f>
@@ -10333,7 +10333,7 @@
       </c>
       <c r="G18" s="38">
         <f>_xll.qlRateHelperEarliestDate($D18)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H18" s="37">
         <f>_xll.qlRateHelperLatestDate($D18)</f>
@@ -10363,11 +10363,11 @@
       </c>
       <c r="G19" s="38">
         <f>_xll.qlRateHelperEarliestDate($D19)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H19" s="37">
         <f>_xll.qlRateHelperLatestDate($D19)</f>
-        <v>43850</v>
+        <v>43851</v>
       </c>
       <c r="I19" s="32" t="e">
         <v>#NUM!</v>
@@ -10393,11 +10393,11 @@
       </c>
       <c r="G20" s="38">
         <f>_xll.qlRateHelperEarliestDate($D20)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H20" s="37">
         <f>_xll.qlRateHelperLatestDate($D20)</f>
-        <v>44216</v>
+        <v>44217</v>
       </c>
       <c r="I20" s="32" t="e">
         <v>#NUM!</v>
@@ -10423,11 +10423,11 @@
       </c>
       <c r="G21" s="38">
         <f>_xll.qlRateHelperEarliestDate($D21)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H21" s="37">
         <f>_xll.qlRateHelperLatestDate($D21)</f>
-        <v>44581</v>
+        <v>44582</v>
       </c>
       <c r="I21" s="32" t="e">
         <v>#NUM!</v>
@@ -10453,11 +10453,11 @@
       </c>
       <c r="G22" s="38">
         <f>_xll.qlRateHelperEarliestDate($D22)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H22" s="37">
         <f>_xll.qlRateHelperLatestDate($D22)</f>
-        <v>44946</v>
+        <v>44949</v>
       </c>
       <c r="I22" s="32" t="e">
         <v>#NUM!</v>
@@ -10483,7 +10483,7 @@
       </c>
       <c r="G23" s="38">
         <f>_xll.qlRateHelperEarliestDate($D23)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H23" s="37">
         <f>_xll.qlRateHelperLatestDate($D23)</f>
@@ -10513,11 +10513,11 @@
       </c>
       <c r="G24" s="38">
         <f>_xll.qlRateHelperEarliestDate($D24)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H24" s="37">
         <f>_xll.qlRateHelperLatestDate($D24)</f>
-        <v>46042</v>
+        <v>46043</v>
       </c>
       <c r="I24" s="32" t="e">
         <v>#NUM!</v>
@@ -10543,7 +10543,7 @@
       </c>
       <c r="G25" s="38">
         <f>_xll.qlRateHelperEarliestDate($D25)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H25" s="37">
         <f>_xll.qlRateHelperLatestDate($D25)</f>
@@ -10573,11 +10573,11 @@
       </c>
       <c r="G26" s="38">
         <f>_xll.qlRateHelperEarliestDate($D26)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H26" s="37">
         <f>_xll.qlRateHelperLatestDate($D26)</f>
-        <v>48964</v>
+        <v>48967</v>
       </c>
       <c r="I26" s="32" t="e">
         <v>#NUM!</v>
@@ -10603,11 +10603,11 @@
       </c>
       <c r="G27" s="38">
         <f>_xll.qlRateHelperEarliestDate($D27)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H27" s="37">
         <f>_xll.qlRateHelperLatestDate($D27)</f>
-        <v>50790</v>
+        <v>50791</v>
       </c>
       <c r="I27" s="32" t="e">
         <v>#NUM!</v>
@@ -10633,11 +10633,11 @@
       </c>
       <c r="G28" s="38">
         <f>_xll.qlRateHelperEarliestDate($D28)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H28" s="37">
         <f>_xll.qlRateHelperLatestDate($D28)</f>
-        <v>52616</v>
+        <v>52617</v>
       </c>
       <c r="I28" s="32" t="e">
         <v>#NUM!</v>
@@ -10663,11 +10663,11 @@
       </c>
       <c r="G29" s="38">
         <f>_xll.qlRateHelperEarliestDate($D29)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H29" s="37">
         <f>_xll.qlRateHelperLatestDate($D29)</f>
-        <v>54443</v>
+        <v>54444</v>
       </c>
       <c r="I29" s="32" t="e">
         <v>#NUM!</v>
@@ -10693,11 +10693,11 @@
       </c>
       <c r="G30" s="38">
         <f>_xll.qlRateHelperEarliestDate($D30)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H30" s="37">
         <f>_xll.qlRateHelperLatestDate($D30)</f>
-        <v>56269</v>
+        <v>56270</v>
       </c>
       <c r="I30" s="32" t="e">
         <v>#NUM!</v>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="G31" s="38">
         <f>_xll.qlRateHelperEarliestDate($D31)</f>
-        <v>41659</v>
+        <v>41660</v>
       </c>
       <c r="H31" s="37">
         <f>_xll.qlRateHelperLatestDate($D31)</f>
@@ -13111,7 +13111,7 @@
       </c>
       <c r="F3" s="101" t="str">
         <f>_xll.qlDepositRateHelper2(E3,D3,"1d",2,"target","following",FALSE,"act/360",Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_SND#0002</v>
+        <v>USD_YC6MRH_SND#0000</v>
       </c>
       <c r="G3" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F3)</f>
@@ -13138,7 +13138,7 @@
       </c>
       <c r="F4" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E4,D4,C4,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_SWD#0002</v>
+        <v>USD_YC6MRH_SWD#0000</v>
       </c>
       <c r="G4" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F4)</f>
@@ -13165,7 +13165,7 @@
       </c>
       <c r="F5" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E5,D5,C5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2WD#0002</v>
+        <v>USD_YC6MRH_2WD#0000</v>
       </c>
       <c r="G5" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F5)</f>
@@ -13192,7 +13192,7 @@
       </c>
       <c r="F6" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E6,D6,C6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3WD#0002</v>
+        <v>USD_YC6MRH_3WD#0000</v>
       </c>
       <c r="G6" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F6)</f>
@@ -13219,7 +13219,7 @@
       </c>
       <c r="F7" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E7,D7,C7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_1MD#0002</v>
+        <v>USD_YC6MRH_1MD#0000</v>
       </c>
       <c r="G7" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F7)</f>
@@ -13246,7 +13246,7 @@
       </c>
       <c r="F8" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E8,D8,C8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2MD#0002</v>
+        <v>USD_YC6MRH_2MD#0000</v>
       </c>
       <c r="G8" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F8)</f>
@@ -13273,7 +13273,7 @@
       </c>
       <c r="F9" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E9,D9,C9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3MD#0002</v>
+        <v>USD_YC6MRH_3MD#0000</v>
       </c>
       <c r="G9" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F9)</f>
@@ -13300,7 +13300,7 @@
       </c>
       <c r="F10" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E10,D10,C10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_4MD#0002</v>
+        <v>USD_YC6MRH_4MD#0000</v>
       </c>
       <c r="G10" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F10)</f>
@@ -13327,7 +13327,7 @@
       </c>
       <c r="F11" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E11,D11,C11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_5MD#0002</v>
+        <v>USD_YC6MRH_5MD#0000</v>
       </c>
       <c r="G11" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F11)</f>
@@ -13354,7 +13354,7 @@
       </c>
       <c r="F12" s="95" t="str">
         <f>_xll.qlDepositRateHelper(E12,D12,C12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_6MD#0002</v>
+        <v>USD_YC6MRH_6MD#0000</v>
       </c>
       <c r="G12" s="94" t="str">
         <f>_xll.ohRangeRetrieveError(F12)</f>
@@ -13447,7 +13447,7 @@
       </c>
       <c r="J2" s="147" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I2)</f>
-        <v>ohObjectSave - operToVectorImpl: error converting parameter 'ObjectList' to type 'class std::basic_string&lt;char,struct std::char_traits&lt;char&gt;,class std::allocator&lt;char&gt; &gt;' : Unable to convert type 'struct ObjectHandler::empty_property_tag' to type 'class s</v>
+        <v/>
       </c>
       <c r="K2" s="93"/>
     </row>
@@ -13484,7 +13484,7 @@
       </c>
       <c r="J3" s="147" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I3)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USDT6F1_Quote'</v>
+        <v/>
       </c>
       <c r="K3" s="93"/>
     </row>
@@ -13521,7 +13521,7 @@
       </c>
       <c r="J4" s="143" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I4)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USDTOM6F1_Quote'</v>
+        <v/>
       </c>
       <c r="K4" s="93"/>
     </row>
@@ -13555,7 +13555,7 @@
       </c>
       <c r="I5" s="139" t="str">
         <f>_xll.qlFraRateHelper(H5,G5,B5,E5,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_1x7F#0002</v>
+        <v>USD_YC6MRH_1x7F#0000</v>
       </c>
       <c r="J5" s="138" t="str">
         <f>_xll.ohRangeRetrieveError(I5)</f>
@@ -13593,7 +13593,7 @@
       </c>
       <c r="I6" s="134" t="str">
         <f>_xll.qlFraRateHelper(H6,G6,B6,E6,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_2x8F#0002</v>
+        <v>USD_YC6MRH_2x8F#0000</v>
       </c>
       <c r="J6" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I6)</f>
@@ -13631,7 +13631,7 @@
       </c>
       <c r="I7" s="134" t="str">
         <f>_xll.qlFraRateHelper(H7,G7,B7,E7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_3x9F#0002</v>
+        <v>USD_YC6MRH_3x9F#0000</v>
       </c>
       <c r="J7" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I7)</f>
@@ -13669,7 +13669,7 @@
       </c>
       <c r="I8" s="134" t="str">
         <f>_xll.qlFraRateHelper(H8,G8,B8,E8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_4x10F#0002</v>
+        <v>USD_YC6MRH_4x10F#0000</v>
       </c>
       <c r="J8" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I8)</f>
@@ -13707,7 +13707,7 @@
       </c>
       <c r="I9" s="134" t="str">
         <f>_xll.qlFraRateHelper(H9,G9,B9,E9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_5x11F#0002</v>
+        <v>USD_YC6MRH_5x11F#0000</v>
       </c>
       <c r="J9" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
@@ -13745,7 +13745,7 @@
       </c>
       <c r="I10" s="134" t="str">
         <f>_xll.qlFraRateHelper(H10,G10,B10,E10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_6x12F#0002</v>
+        <v>USD_YC6MRH_6x12F#0000</v>
       </c>
       <c r="J10" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
@@ -13787,7 +13787,7 @@
       </c>
       <c r="J11" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I11)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD7x13F_Quote'</v>
+        <v/>
       </c>
       <c r="K11" s="93"/>
     </row>
@@ -13825,7 +13825,7 @@
       </c>
       <c r="J12" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I12)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD8x14F_Quote'</v>
+        <v/>
       </c>
       <c r="K12" s="93"/>
     </row>
@@ -13863,7 +13863,7 @@
       </c>
       <c r="J13" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I13)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD9x15F_Quote'</v>
+        <v/>
       </c>
       <c r="K13" s="93"/>
     </row>
@@ -13901,7 +13901,7 @@
       </c>
       <c r="J14" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I14)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD10x16F_Quote'</v>
+        <v/>
       </c>
       <c r="K14" s="93"/>
     </row>
@@ -13939,7 +13939,7 @@
       </c>
       <c r="J15" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I15)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD11x17F_Quote'</v>
+        <v/>
       </c>
       <c r="K15" s="93"/>
     </row>
@@ -13973,7 +13973,7 @@
       </c>
       <c r="I16" s="134" t="str">
         <f>_xll.qlFraRateHelper(H16,G16,B16,E16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_12x18F#0002</v>
+        <v>USD_YC6MRH_12x18F#0000</v>
       </c>
       <c r="J16" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
@@ -14015,7 +14015,7 @@
       </c>
       <c r="J17" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I17)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD13x19F_Quote'</v>
+        <v/>
       </c>
       <c r="K17" s="93"/>
     </row>
@@ -14053,7 +14053,7 @@
       </c>
       <c r="J18" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I18)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD14x20F_Quote'</v>
+        <v/>
       </c>
       <c r="K18" s="93"/>
     </row>
@@ -14091,7 +14091,7 @@
       </c>
       <c r="J19" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I19)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD15x21F_Quote'</v>
+        <v/>
       </c>
       <c r="K19" s="93"/>
     </row>
@@ -14129,7 +14129,7 @@
       </c>
       <c r="J20" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I20)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD16x22F_Quote'</v>
+        <v/>
       </c>
       <c r="K20" s="93"/>
     </row>
@@ -14167,7 +14167,7 @@
       </c>
       <c r="J21" s="133" t="str">
         <f ca="1">_xll.ohRangeRetrieveError(I21)</f>
-        <v>qlFraRateHelper - Error converting parameter 'Rate' : 'ObjectHandler error: attempt to retrieve object with unknown ID 'USD17x23F_Quote'</v>
+        <v/>
       </c>
       <c r="K21" s="93"/>
     </row>
@@ -14201,7 +14201,7 @@
       </c>
       <c r="I22" s="134" t="str">
         <f>_xll.qlFraRateHelper(H22,G22,B22,E22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_18x24F#0002</v>
+        <v>USD_YC6MRH_18x24F#0000</v>
       </c>
       <c r="J22" s="133" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
@@ -14240,7 +14240,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -14365,7 +14365,7 @@
       </c>
       <c r="L4" s="180" t="str">
         <f>IF(UPPER(FamilyName)="IBOR",_xll.qlEuribor($K4,$J$2,,Permanent,Trigger,ObjectOverwrite),IF(UPPER(FamilyName)="LIBOR",_xll.qlLibor($K4,Currency,$J$2,,Permanent,Trigger,ObjectOverwrite),"--"))</f>
-        <v>USD_YC6MRH_AM6LBASIS_Libor6M#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS_Libor6M#0000</v>
       </c>
       <c r="M4" s="179" t="str">
         <f>_xll.ohRangeRetrieveError(L4)</f>
@@ -14429,7 +14429,7 @@
       </c>
       <c r="L6" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K6,$J6,$C6,Calendar,$F6,$G6,$H6,$L$4,$I6,B6,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS1Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS1Y#0000</v>
       </c>
       <c r="M6" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L6)</f>
@@ -14616,7 +14616,7 @@
       </c>
       <c r="L10" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K10,$J10,$C10,Calendar,$F10,$G10,$H10,$L$4,$I10,B10,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS2Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS2Y#0000</v>
       </c>
       <c r="M10" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -14678,7 +14678,7 @@
       </c>
       <c r="L11" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K11,$J11,$C11,Calendar,$F11,$G11,$H11,$L$4,$I11,B11,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS3Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS3Y#0000</v>
       </c>
       <c r="M11" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -14736,7 +14736,7 @@
       </c>
       <c r="L12" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K12,$J12,$C12,Calendar,$F12,$G12,$H12,$L$4,$I12,B12,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS4Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS4Y#0000</v>
       </c>
       <c r="M12" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -14794,7 +14794,7 @@
       </c>
       <c r="L13" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K13,$J13,$C13,Calendar,$F13,$G13,$H13,$L$4,$I13,B13,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS5Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS5Y#0000</v>
       </c>
       <c r="M13" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -14852,7 +14852,7 @@
       </c>
       <c r="L14" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K14,$J14,$C14,Calendar,$F14,$G14,$H14,$L$4,$I14,B14,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS6Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS6Y#0000</v>
       </c>
       <c r="M14" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -14910,7 +14910,7 @@
       </c>
       <c r="L15" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K15,$J15,$C15,Calendar,$F15,$G15,$H15,$L$4,$I15,B15,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS7Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS7Y#0000</v>
       </c>
       <c r="M15" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L15)</f>
@@ -14962,7 +14962,7 @@
       </c>
       <c r="L16" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K16,$J16,$C16,Calendar,$F16,$G16,$H16,$L$4,$I16,B16,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS8Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS8Y#0000</v>
       </c>
       <c r="M16" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L16)</f>
@@ -15011,7 +15011,7 @@
       </c>
       <c r="L17" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K17,$J17,$C17,Calendar,$F17,$G17,$H17,$L$4,$I17,B17,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS9Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS9Y#0000</v>
       </c>
       <c r="M17" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L17)</f>
@@ -15060,7 +15060,7 @@
       </c>
       <c r="L18" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K18,$J18,$C18,Calendar,$F18,$G18,$H18,$L$4,$I18,B18,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS10Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS10Y#0000</v>
       </c>
       <c r="M18" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L18)</f>
@@ -15109,7 +15109,7 @@
       </c>
       <c r="L19" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K19,$J19,$C19,Calendar,$F19,$G19,$H19,$L$4,$I19,B19,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS11Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS11Y#0000</v>
       </c>
       <c r="M19" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L19)</f>
@@ -15158,7 +15158,7 @@
       </c>
       <c r="L20" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K20,$J20,$C20,Calendar,$F20,$G20,$H20,$L$4,$I20,B20,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS12Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS12Y#0000</v>
       </c>
       <c r="M20" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L20)</f>
@@ -15207,7 +15207,7 @@
       </c>
       <c r="L21" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K21,$J21,$C21,Calendar,$F21,$G21,$H21,$L$4,$I21,B21,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS13Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS13Y#0000</v>
       </c>
       <c r="M21" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L21)</f>
@@ -15256,7 +15256,7 @@
       </c>
       <c r="L22" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K22,$J22,$C22,Calendar,$F22,$G22,$H22,$L$4,$I22,B22,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS14Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS14Y#0000</v>
       </c>
       <c r="M22" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L22)</f>
@@ -15305,7 +15305,7 @@
       </c>
       <c r="L23" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K23,$J23,$C23,Calendar,$F23,$G23,$H23,$L$4,$I23,B23,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS15Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS15Y#0000</v>
       </c>
       <c r="M23" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L23)</f>
@@ -15354,7 +15354,7 @@
       </c>
       <c r="L24" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K24,$J24,$C24,Calendar,$F24,$G24,$H24,$L$4,$I24,B24,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS16Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS16Y#0000</v>
       </c>
       <c r="M24" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L24)</f>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="L25" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K25,$J25,$C25,Calendar,$F25,$G25,$H25,$L$4,$I25,B25,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS17Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS17Y#0000</v>
       </c>
       <c r="M25" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L25)</f>
@@ -15452,7 +15452,7 @@
       </c>
       <c r="L26" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K26,$J26,$C26,Calendar,$F26,$G26,$H26,$L$4,$I26,B26,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS18Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS18Y#0000</v>
       </c>
       <c r="M26" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L26)</f>
@@ -15501,7 +15501,7 @@
       </c>
       <c r="L27" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K27,$J27,$C27,Calendar,$F27,$G27,$H27,$L$4,$I27,B27,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS19Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS19Y#0000</v>
       </c>
       <c r="M27" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L27)</f>
@@ -15550,7 +15550,7 @@
       </c>
       <c r="L28" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K28,$J28,$C28,Calendar,$F28,$G28,$H28,$L$4,$I28,B28,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS20Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS20Y#0000</v>
       </c>
       <c r="M28" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L28)</f>
@@ -15599,7 +15599,7 @@
       </c>
       <c r="L29" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K29,$J29,$C29,Calendar,$F29,$G29,$H29,$L$4,$I29,B29,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS21Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS21Y#0000</v>
       </c>
       <c r="M29" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L29)</f>
@@ -15648,7 +15648,7 @@
       </c>
       <c r="L30" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K30,$J30,$C30,Calendar,$F30,$G30,$H30,$L$4,$I30,B30,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS22Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS22Y#0000</v>
       </c>
       <c r="M30" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L30)</f>
@@ -15697,7 +15697,7 @@
       </c>
       <c r="L31" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K31,$J31,$C31,Calendar,$F31,$G31,$H31,$L$4,$I31,B31,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS23Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS23Y#0000</v>
       </c>
       <c r="M31" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L31)</f>
@@ -15746,7 +15746,7 @@
       </c>
       <c r="L32" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K32,$J32,$C32,Calendar,$F32,$G32,$H32,$L$4,$I32,B32,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS24Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS24Y#0000</v>
       </c>
       <c r="M32" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L32)</f>
@@ -15795,7 +15795,7 @@
       </c>
       <c r="L33" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K33,$J33,$C33,Calendar,$F33,$G33,$H33,$L$4,$I33,B33,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS25Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS25Y#0000</v>
       </c>
       <c r="M33" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L33)</f>
@@ -15844,7 +15844,7 @@
       </c>
       <c r="L34" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K34,$J34,$C34,Calendar,$F34,$G34,$H34,$L$4,$I34,B34,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS26Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS26Y#0000</v>
       </c>
       <c r="M34" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L34)</f>
@@ -15893,7 +15893,7 @@
       </c>
       <c r="L35" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K35,$J35,$C35,Calendar,$F35,$G35,$H35,$L$4,$I35,B35,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS27Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS27Y#0000</v>
       </c>
       <c r="M35" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L35)</f>
@@ -15942,7 +15942,7 @@
       </c>
       <c r="L36" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K36,$J36,$C36,Calendar,$F36,$G36,$H36,$L$4,$I36,B36,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS28Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS28Y#0000</v>
       </c>
       <c r="M36" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L36)</f>
@@ -15991,7 +15991,7 @@
       </c>
       <c r="L37" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K37,$J37,$C37,Calendar,$F37,$G37,$H37,$L$4,$I37,B37,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS29Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS29Y#0000</v>
       </c>
       <c r="M37" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L37)</f>
@@ -16040,7 +16040,7 @@
       </c>
       <c r="L38" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K38,$J38,$C38,Calendar,$F38,$G38,$H38,$L$4,$I38,B38,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS30Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS30Y#0000</v>
       </c>
       <c r="M38" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L38)</f>
@@ -16089,7 +16089,7 @@
       </c>
       <c r="L39" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K39,$J39,$C39,Calendar,$F39,$G39,$H39,$L$4,$I39,B39,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS35Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS35Y#0000</v>
       </c>
       <c r="M39" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L39)</f>
@@ -16138,7 +16138,7 @@
       </c>
       <c r="L40" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K40,$J40,$C40,Calendar,$F40,$G40,$H40,$L$4,$I40,B40,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS40Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS40Y#0000</v>
       </c>
       <c r="M40" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L40)</f>
@@ -16187,7 +16187,7 @@
       </c>
       <c r="L41" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K41,$J41,$C41,Calendar,$F41,$G41,$H41,$L$4,$I41,B41,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS50Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS50Y#0000</v>
       </c>
       <c r="M41" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L41)</f>
@@ -16236,7 +16236,7 @@
       </c>
       <c r="L42" s="164" t="str">
         <f>_xll.qlSwapRateHelper2(K42,$J42,$C42,Calendar,$F42,$G42,$H42,$L$4,$I42,B42,DiscountingCurve,Permanent,,ObjectOverwrite)</f>
-        <v>USD_YC6MRH_AM6LBASIS60Y#0002</v>
+        <v>USD_YC6MRH_AM6LBASIS60Y#0000</v>
       </c>
       <c r="M42" s="163" t="str">
         <f>_xll.ohRangeRetrieveError(L42)</f>

</xml_diff>